<commit_message>
feat: update all infomation for each employee
</commit_message>
<xml_diff>
--- a/public/documents/payslip.xlsx
+++ b/public/documents/payslip.xlsx
@@ -27,27 +27,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="48">
   <si>
     <t>CÔNG TY TNHH HIGHWAN TECH VIETNAM</t>
   </si>
   <si>
-    <t>BẢNG LƯƠNG CÁ NHÂN THÁNG 12-2025</t>
-  </si>
-  <si>
-    <t>Từ/From 26/11/2025 đến/to 25/12/2025</t>
-  </si>
-  <si>
-    <t>Name/ Tên:</t>
+    <t>BẢNG LƯƠNG CÁ NHÂN THÁNG 12/2025</t>
+  </si>
+  <si>
+    <t>Từ 26/11/2025 đến 25/12/2025</t>
+  </si>
+  <si>
+    <t>Họ và tên:</t>
   </si>
   <si>
     <t>Trần Thị Bé</t>
   </si>
   <si>
-    <t>Brithday:</t>
-  </si>
-  <si>
-    <t>Department/ Bộ phận:</t>
+    <t>Ngày sinh:</t>
+  </si>
+  <si>
+    <t>Bộ phận:</t>
   </si>
   <si>
     <t>Công nhân/sản xuất</t>
@@ -56,8 +56,7 @@
     <t>Code/ Mã:</t>
   </si>
   <si>
-    <t>THÔNG TIN CƠ BẢN
-BASIC INFORMATION</t>
+    <t>THÔNG TIN CƠ BẢN</t>
   </si>
   <si>
     <t>Description/Mô tả</t>
@@ -66,49 +65,46 @@
     <t>Kết quả/ Result</t>
   </si>
   <si>
-    <t>Tổng số ngày làm việc/tháng</t>
+    <t>Số ngày làm việc trong tháng</t>
   </si>
   <si>
     <t>Ngày</t>
   </si>
   <si>
-    <t>Nghỉ lễ, kết hôn, tang chế/ Holiday, Married, Mourning</t>
-  </si>
-  <si>
-    <t>Nghỉ phép/ Annual leave</t>
-  </si>
-  <si>
-    <t>Nghỉ ốm, Thai sản/ Sick, Maternity leave</t>
-  </si>
-  <si>
-    <t>Nghỉ 70% lương/ Unpaid leave</t>
-  </si>
-  <si>
-    <t>Nghỉ không lương/ Unpaid leave</t>
-  </si>
-  <si>
-    <t>Tổng ngày lương được trả/ Total paid days</t>
-  </si>
-  <si>
-    <t>Tăng ca 150%/ OT 150%</t>
+    <t>Nghỉ lễ, kết hôn, tang chế</t>
+  </si>
+  <si>
+    <t>Nghỉ phép năm</t>
+  </si>
+  <si>
+    <t>Nghỉ ốm, Thai sản</t>
+  </si>
+  <si>
+    <t>Nghỉ không lương</t>
+  </si>
+  <si>
+    <t>Số ngày làm việc thực tế (ngày)</t>
+  </si>
+  <si>
+    <t>Tăng ca 150%</t>
   </si>
   <si>
     <t>Giờ</t>
   </si>
   <si>
-    <t>Tăng ca 200%/ OT 200%</t>
-  </si>
-  <si>
-    <t>Tăng ca 300%/ OT 300%</t>
-  </si>
-  <si>
-    <t>Tăng ca 210%/ OT 210%</t>
-  </si>
-  <si>
-    <t>Tăng ca 270%/ OT 270%</t>
-  </si>
-  <si>
-    <t>Tăng ca 390%/ OT 390%</t>
+    <t>Tăng ca 200%</t>
+  </si>
+  <si>
+    <t>Tăng ca 300%</t>
+  </si>
+  <si>
+    <t>Tăng ca 210%</t>
+  </si>
+  <si>
+    <t>Tăng ca 270%</t>
+  </si>
+  <si>
+    <t>Tăng ca 390%</t>
   </si>
   <si>
     <t>Lương cơ bản</t>
@@ -117,62 +113,58 @@
     <t>VND</t>
   </si>
   <si>
-    <t>Phụ cấp đi lại, nhà ở/ Other allowance</t>
-  </si>
-  <si>
-    <t>Tổng lương/ Total Salary</t>
-  </si>
-  <si>
-    <t>LƯƠNG, THUẾ
-SALARY &amp; TAX CALCULATION</t>
+    <t>Hỗ trợ xăng xe, nhà ở</t>
+  </si>
+  <si>
+    <t>Tổng lương</t>
+  </si>
+  <si>
+    <t>LƯƠNG, THUẾ</t>
   </si>
   <si>
     <t>Các khoảng thu</t>
   </si>
   <si>
-    <t>Đi trễ, về sớm/ Come late, Leave early</t>
+    <t>Tiền điện thoại</t>
+  </si>
+  <si>
+    <t>Tổng tiền tăng ca</t>
+  </si>
+  <si>
+    <t>Tổng tiền cơm tăng ca</t>
+  </si>
+  <si>
+    <t>Tổng tiền cơm trưa</t>
+  </si>
+  <si>
+    <t>Phí gia công</t>
+  </si>
+  <si>
+    <t>Thưởng Tết</t>
+  </si>
+  <si>
+    <t>Tổng thu nhập</t>
+  </si>
+  <si>
+    <t>Các khoảng khấu trừ</t>
+  </si>
+  <si>
+    <t>Tổng BHXH</t>
+  </si>
+  <si>
+    <t>Công đoàn</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>Chuyên cần/ Diligence</t>
-  </si>
-  <si>
-    <t>Tăng ca/OT</t>
-  </si>
-  <si>
-    <t>Tiền cơm tăng ca</t>
-  </si>
-  <si>
-    <t>Tiền cơm hành chánh/ Meal allowance</t>
-  </si>
-  <si>
-    <t>Phép năm còn lại/ Annual leave remain</t>
-  </si>
-  <si>
-    <t>Điều chỉnh khác/ Other adjust</t>
-  </si>
-  <si>
-    <t>Tổng thu nhập/ Salary</t>
-  </si>
-  <si>
-    <t>Các khoảng khấu trừ</t>
-  </si>
-  <si>
-    <t>BHXH-BHYT-BHTN (10.5%) / Social Insurance</t>
-  </si>
-  <si>
-    <t>Công đoàn/ Trade Union</t>
-  </si>
-  <si>
-    <t>Thuế TNCN/ Personal Income Tax</t>
-  </si>
-  <si>
-    <t>Tổng khấu trừ/ Deduction</t>
-  </si>
-  <si>
-    <t>Lương thực nhận/ Actual salary</t>
+    <t>Thuế TNCN</t>
+  </si>
+  <si>
+    <t>Tổng khấu trừ</t>
+  </si>
+  <si>
+    <t>Lương thực nhận</t>
   </si>
   <si>
     <t>Người nhận</t>
@@ -185,14 +177,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="7">
+  <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0\ _₫_-;\-* #,##0\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -1254,7 +1244,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1307,9 +1297,7 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1329,27 +1317,21 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="177" fontId="6" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="177" fontId="7" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1387,7 +1369,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1715,18 +1708,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="3.42592592592593" customWidth="1"/>
-    <col min="2" max="2" width="13.4259259259259" customWidth="1"/>
-    <col min="3" max="3" width="22.1018518518519" customWidth="1"/>
-    <col min="4" max="4" width="29.1666666666667" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7777777777778" customWidth="1"/>
+    <col min="3" max="3" width="11.7777777777778" customWidth="1"/>
+    <col min="4" max="4" width="30.7777777777778" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.8518518518519" style="1" customWidth="1"/>
     <col min="6" max="6" width="6.57407407407407" customWidth="1"/>
     <col min="7" max="7" width="4.13888888888889" customWidth="1"/>
@@ -1799,12 +1792,12 @@
     </row>
     <row r="7" ht="18" customHeight="1" spans="1:7">
       <c r="A7" s="6"/>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
       <c r="G7" s="8"/>
     </row>
     <row r="8" ht="18" customHeight="1" spans="1:7">
@@ -1894,11 +1887,13 @@
     <row r="14" s="1" customFormat="1" ht="18" customHeight="1" spans="1:8">
       <c r="A14" s="6"/>
       <c r="B14" s="17"/>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="27"/>
-      <c r="E14" s="28"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24">
+        <v>2</v>
+      </c>
       <c r="F14" s="25" t="s">
         <v>13</v>
       </c>
@@ -1908,14 +1903,14 @@
     <row r="15" s="1" customFormat="1" ht="18" customHeight="1" spans="1:8">
       <c r="A15" s="6"/>
       <c r="B15" s="17"/>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="29">
-        <v>2</v>
-      </c>
-      <c r="F15" s="25" t="s">
+      <c r="D15" s="27"/>
+      <c r="E15" s="28">
+        <v>24</v>
+      </c>
+      <c r="F15" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G15" s="8"/>
@@ -1924,34 +1919,33 @@
     <row r="16" s="1" customFormat="1" ht="18" customHeight="1" spans="1:8">
       <c r="A16" s="6"/>
       <c r="B16" s="17"/>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="27"/>
-      <c r="E16" s="30">
-        <v>24</v>
-      </c>
-      <c r="F16" s="31" t="s">
-        <v>13</v>
+      <c r="D16" s="23"/>
+      <c r="E16" s="24">
+        <v>32</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>20</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16"/>
     </row>
-    <row r="17" s="1" customFormat="1" ht="18" customHeight="1" spans="1:8">
+    <row r="17" ht="18" customHeight="1" spans="1:7">
       <c r="A17" s="6"/>
       <c r="B17" s="17"/>
       <c r="C17" s="22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D17" s="23"/>
       <c r="E17" s="24">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G17" s="8"/>
-      <c r="H17"/>
     </row>
     <row r="18" ht="18" customHeight="1" spans="1:7">
       <c r="A18" s="6"/>
@@ -1964,7 +1958,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G18" s="8"/>
     </row>
@@ -1979,7 +1973,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G19" s="8"/>
     </row>
@@ -1994,7 +1988,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G20" s="8"/>
     </row>
@@ -2009,7 +2003,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G21" s="8"/>
     </row>
@@ -2021,10 +2015,10 @@
       </c>
       <c r="D22" s="23"/>
       <c r="E22" s="24">
-        <v>0</v>
+        <v>5000000</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="G22" s="8"/>
     </row>
@@ -2032,330 +2026,296 @@
       <c r="A23" s="6"/>
       <c r="B23" s="17"/>
       <c r="C23" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="23"/>
+      <c r="E23" s="30">
+        <v>1500000</v>
+      </c>
+      <c r="F23" s="25" t="s">
         <v>27</v>
-      </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="24">
-        <v>5000000</v>
-      </c>
-      <c r="F23" s="25" t="s">
-        <v>28</v>
       </c>
       <c r="G23" s="8"/>
     </row>
     <row r="24" ht="18" customHeight="1" spans="1:7">
       <c r="A24" s="6"/>
       <c r="B24" s="17"/>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="23"/>
-      <c r="E24" s="32">
-        <v>1500000</v>
-      </c>
-      <c r="F24" s="25" t="s">
-        <v>28</v>
+      <c r="D24" s="32"/>
+      <c r="E24" s="33">
+        <v>6000000</v>
+      </c>
+      <c r="F24" s="34" t="s">
+        <v>27</v>
       </c>
       <c r="G24" s="8"/>
     </row>
     <row r="25" ht="18" customHeight="1" spans="1:7">
       <c r="A25" s="6"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="33" t="s">
+      <c r="B25" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="34"/>
-      <c r="E25" s="35">
-        <v>6000000</v>
-      </c>
-      <c r="F25" s="36" t="s">
-        <v>28</v>
-      </c>
+      <c r="C25" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="38"/>
       <c r="G25" s="8"/>
     </row>
     <row r="26" ht="18" customHeight="1" spans="1:7">
       <c r="A26" s="6"/>
-      <c r="B26" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="38" t="s">
+      <c r="B26" s="39"/>
+      <c r="C26" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="39"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="41"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="24">
+        <v>461538</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>27</v>
+      </c>
       <c r="G26" s="8"/>
     </row>
     <row r="27" ht="18" customHeight="1" spans="1:7">
       <c r="A27" s="6"/>
-      <c r="B27" s="42"/>
+      <c r="B27" s="39"/>
       <c r="C27" s="22" t="s">
         <v>33</v>
       </c>
       <c r="D27" s="23"/>
-      <c r="E27" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="F27" s="43" t="s">
-        <v>28</v>
+      <c r="E27" s="24">
+        <v>1153846</v>
+      </c>
+      <c r="F27" s="40" t="s">
+        <v>27</v>
       </c>
       <c r="G27" s="8"/>
     </row>
     <row r="28" ht="18" customHeight="1" spans="1:7">
       <c r="A28" s="6"/>
-      <c r="B28" s="42"/>
+      <c r="B28" s="39"/>
       <c r="C28" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D28" s="23"/>
       <c r="E28" s="24">
-        <v>461538</v>
-      </c>
-      <c r="F28" s="25" t="s">
-        <v>28</v>
+        <v>240000</v>
+      </c>
+      <c r="F28" s="40" t="s">
+        <v>27</v>
       </c>
       <c r="G28" s="8"/>
     </row>
     <row r="29" ht="18" customHeight="1" spans="1:7">
       <c r="A29" s="6"/>
-      <c r="B29" s="42"/>
+      <c r="B29" s="39"/>
       <c r="C29" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D29" s="23"/>
       <c r="E29" s="24">
-        <v>1153846</v>
-      </c>
-      <c r="F29" s="44" t="s">
-        <v>28</v>
+        <v>690000</v>
+      </c>
+      <c r="F29" s="40" t="s">
+        <v>27</v>
       </c>
       <c r="G29" s="8"/>
     </row>
     <row r="30" ht="18" customHeight="1" spans="1:7">
       <c r="A30" s="6"/>
-      <c r="B30" s="42"/>
+      <c r="B30" s="39"/>
       <c r="C30" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D30" s="23"/>
-      <c r="E30" s="24">
-        <v>240000</v>
-      </c>
-      <c r="F30" s="44" t="s">
-        <v>28</v>
+      <c r="E30" s="41"/>
+      <c r="F30" s="40" t="s">
+        <v>27</v>
       </c>
       <c r="G30" s="8"/>
     </row>
     <row r="31" ht="18" customHeight="1" spans="1:7">
       <c r="A31" s="6"/>
-      <c r="B31" s="42"/>
-      <c r="C31" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="24">
-        <v>690000</v>
-      </c>
-      <c r="F31" s="44" t="s">
-        <v>28</v>
+      <c r="B31" s="39"/>
+      <c r="C31" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="43"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="40" t="s">
+        <v>27</v>
       </c>
       <c r="G31" s="8"/>
     </row>
     <row r="32" ht="18" customHeight="1" spans="1:7">
       <c r="A32" s="6"/>
-      <c r="B32" s="42"/>
-      <c r="C32" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32" s="23"/>
-      <c r="E32" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="F32" s="44" t="s">
-        <v>28</v>
+      <c r="B32" s="39"/>
+      <c r="C32" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="32"/>
+      <c r="E32" s="45">
+        <v>2545385</v>
+      </c>
+      <c r="F32" s="40" t="s">
+        <v>27</v>
       </c>
       <c r="G32" s="8"/>
     </row>
     <row r="33" ht="18" customHeight="1" spans="1:7">
       <c r="A33" s="6"/>
-      <c r="B33" s="42"/>
-      <c r="C33" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" s="23"/>
-      <c r="E33" s="45"/>
-      <c r="F33" s="44" t="s">
-        <v>28</v>
-      </c>
+      <c r="B33" s="39"/>
+      <c r="C33" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="47"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="48"/>
       <c r="G33" s="8"/>
     </row>
     <row r="34" ht="18" customHeight="1" spans="1:7">
       <c r="A34" s="6"/>
-      <c r="B34" s="42"/>
-      <c r="C34" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="D34" s="34"/>
-      <c r="E34" s="46">
-        <v>2545385</v>
-      </c>
-      <c r="F34" s="44" t="s">
-        <v>28</v>
+      <c r="B34" s="39"/>
+      <c r="C34" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" s="50"/>
+      <c r="E34" s="51">
+        <v>525000</v>
+      </c>
+      <c r="F34" s="52" t="s">
+        <v>27</v>
       </c>
       <c r="G34" s="8"/>
     </row>
     <row r="35" ht="18" customHeight="1" spans="1:7">
       <c r="A35" s="6"/>
-      <c r="B35" s="42"/>
-      <c r="C35" s="47" t="s">
+      <c r="B35" s="39"/>
+      <c r="C35" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="23"/>
+      <c r="E35" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="D35" s="48"/>
-      <c r="E35" s="49"/>
-      <c r="F35" s="50"/>
+      <c r="F35" s="54" t="s">
+        <v>27</v>
+      </c>
       <c r="G35" s="8"/>
     </row>
     <row r="36" ht="18" customHeight="1" spans="1:7">
       <c r="A36" s="6"/>
-      <c r="B36" s="42"/>
-      <c r="C36" s="51" t="s">
+      <c r="B36" s="39"/>
+      <c r="C36" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D36" s="52"/>
-      <c r="E36" s="53">
-        <v>525000</v>
+      <c r="D36" s="23"/>
+      <c r="E36" s="53" t="s">
+        <v>42</v>
       </c>
       <c r="F36" s="54" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G36" s="8"/>
     </row>
     <row r="37" ht="18" customHeight="1" spans="1:7">
       <c r="A37" s="6"/>
-      <c r="B37" s="42"/>
-      <c r="C37" s="22" t="s">
+      <c r="B37" s="39"/>
+      <c r="C37" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D37" s="23"/>
-      <c r="E37" s="55" t="s">
-        <v>34</v>
+      <c r="D37" s="32"/>
+      <c r="E37" s="55">
+        <v>525000</v>
       </c>
       <c r="F37" s="56" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G37" s="8"/>
     </row>
     <row r="38" ht="18" customHeight="1" spans="1:7">
       <c r="A38" s="6"/>
-      <c r="B38" s="42"/>
-      <c r="C38" s="22" t="s">
+      <c r="B38" s="57"/>
+      <c r="C38" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="D38" s="23"/>
-      <c r="E38" s="55" t="s">
-        <v>34</v>
-      </c>
-      <c r="F38" s="56" t="s">
-        <v>28</v>
+      <c r="D38" s="59"/>
+      <c r="E38" s="60">
+        <f>E24+E32-E37</f>
+        <v>8020385</v>
+      </c>
+      <c r="F38" s="61" t="s">
+        <v>27</v>
       </c>
       <c r="G38" s="8"/>
     </row>
-    <row r="39" ht="18" customHeight="1" spans="1:7">
+    <row r="39" ht="10" customHeight="1" spans="1:7">
       <c r="A39" s="6"/>
-      <c r="B39" s="42"/>
-      <c r="C39" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" s="34"/>
-      <c r="E39" s="57">
-        <v>525000</v>
-      </c>
-      <c r="F39" s="58" t="s">
-        <v>28</v>
-      </c>
+      <c r="B39" s="62"/>
+      <c r="C39" s="63"/>
+      <c r="D39" s="63"/>
+      <c r="E39" s="64"/>
+      <c r="F39" s="65"/>
       <c r="G39" s="8"/>
     </row>
     <row r="40" ht="18" customHeight="1" spans="1:7">
       <c r="A40" s="6"/>
-      <c r="B40" s="59"/>
-      <c r="C40" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="D40" s="61"/>
-      <c r="E40" s="62">
-        <f>E25+E34-E39+E14</f>
-        <v>8020385</v>
-      </c>
-      <c r="F40" s="63" t="s">
-        <v>28</v>
-      </c>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E40" s="7"/>
       <c r="G40" s="8"/>
     </row>
     <row r="41" ht="18" customHeight="1" spans="1:7">
       <c r="A41" s="6"/>
-      <c r="E41" s="64"/>
+      <c r="C41" s="66"/>
+      <c r="D41" s="66" t="s">
+        <v>47</v>
+      </c>
+      <c r="E41" s="66"/>
       <c r="G41" s="8"/>
     </row>
     <row r="42" ht="18" customHeight="1" spans="1:7">
       <c r="A42" s="6"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E42" s="7"/>
+      <c r="C42" s="67"/>
+      <c r="E42" s="67"/>
       <c r="G42" s="8"/>
     </row>
     <row r="43" ht="18" customHeight="1" spans="1:7">
       <c r="A43" s="6"/>
-      <c r="C43" s="65"/>
-      <c r="D43" s="65" t="s">
-        <v>49</v>
-      </c>
-      <c r="E43" s="65"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
       <c r="G43" s="8"/>
     </row>
     <row r="44" ht="18" customHeight="1" spans="1:7">
       <c r="A44" s="6"/>
-      <c r="C44" s="66"/>
-      <c r="E44" s="66"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="7"/>
       <c r="G44" s="8"/>
     </row>
     <row r="45" ht="18" customHeight="1" spans="1:7">
-      <c r="A45" s="6"/>
-      <c r="C45" s="66"/>
-      <c r="E45" s="66"/>
-      <c r="G45" s="8"/>
-    </row>
-    <row r="46" ht="18" customHeight="1" spans="1:7">
-      <c r="A46" s="6"/>
-      <c r="C46" s="66"/>
-      <c r="E46" s="66"/>
-      <c r="G46" s="8"/>
-    </row>
-    <row r="47" ht="18" customHeight="1" spans="1:7">
-      <c r="A47" s="6"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E47" s="7"/>
-      <c r="G47" s="8"/>
-    </row>
-    <row r="48" ht="18" customHeight="1" spans="1:7">
-      <c r="A48" s="67"/>
-      <c r="B48" s="68"/>
-      <c r="C48" s="68"/>
-      <c r="D48" s="69"/>
-      <c r="E48" s="68"/>
-      <c r="F48" s="68"/>
-      <c r="G48" s="70"/>
+      <c r="A45" s="68"/>
+      <c r="B45" s="69"/>
+      <c r="C45" s="69"/>
+      <c r="D45" s="70"/>
+      <c r="E45" s="69"/>
+      <c r="F45" s="69"/>
+      <c r="G45" s="71"/>
     </row>
   </sheetData>
-  <mergeCells count="43">
+  <mergeCells count="40">
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C7:F7"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E9:F9"/>
@@ -2374,30 +2334,28 @@
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="C26:D26"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C33:F33"/>
     <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="C35:D35"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="B9:B25"/>
-    <mergeCell ref="B26:B40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="B9:B24"/>
+    <mergeCell ref="B25:B38"/>
   </mergeCells>
   <pageMargins left="0.25" right="0" top="0.25" bottom="0" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" scale="70" orientation="portrait"/>
+  <pageSetup paperSize="11" scale="70" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: complete download payslips
</commit_message>
<xml_diff>
--- a/public/documents/payslip.xlsx
+++ b/public/documents/payslip.xlsx
@@ -177,12 +177,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??.0_);_(@_)"/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -1295,9 +1296,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1327,7 +1329,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="177" fontId="6" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="177" fontId="7" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="177" fontId="7" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1860,7 +1861,7 @@
         <v>15</v>
       </c>
       <c r="D12" s="23"/>
-      <c r="E12" s="24">
+      <c r="E12" s="26">
         <v>1</v>
       </c>
       <c r="F12" s="25" t="s">
@@ -1891,7 +1892,7 @@
         <v>17</v>
       </c>
       <c r="D14" s="23"/>
-      <c r="E14" s="24">
+      <c r="E14" s="26">
         <v>2</v>
       </c>
       <c r="F14" s="25" t="s">
@@ -1903,14 +1904,14 @@
     <row r="15" s="1" customFormat="1" ht="18" customHeight="1" spans="1:8">
       <c r="A15" s="6"/>
       <c r="B15" s="17"/>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="27"/>
-      <c r="E15" s="28">
+      <c r="D15" s="28"/>
+      <c r="E15" s="29">
         <v>24</v>
       </c>
-      <c r="F15" s="29" t="s">
+      <c r="F15" s="30" t="s">
         <v>13</v>
       </c>
       <c r="G15" s="8"/>
@@ -2029,7 +2030,7 @@
         <v>28</v>
       </c>
       <c r="D23" s="23"/>
-      <c r="E23" s="30">
+      <c r="E23" s="31">
         <v>1500000</v>
       </c>
       <c r="F23" s="25" t="s">
@@ -2040,34 +2041,34 @@
     <row r="24" ht="18" customHeight="1" spans="1:7">
       <c r="A24" s="6"/>
       <c r="B24" s="17"/>
-      <c r="C24" s="31" t="s">
+      <c r="C24" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="32"/>
-      <c r="E24" s="33">
+      <c r="D24" s="33"/>
+      <c r="E24" s="34">
         <v>6000000</v>
       </c>
-      <c r="F24" s="34" t="s">
+      <c r="F24" s="35" t="s">
         <v>27</v>
       </c>
       <c r="G24" s="8"/>
     </row>
     <row r="25" ht="18" customHeight="1" spans="1:7">
       <c r="A25" s="6"/>
-      <c r="B25" s="35" t="s">
+      <c r="B25" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="36" t="s">
+      <c r="C25" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="39"/>
       <c r="G25" s="8"/>
     </row>
     <row r="26" ht="18" customHeight="1" spans="1:7">
       <c r="A26" s="6"/>
-      <c r="B26" s="39"/>
+      <c r="B26" s="40"/>
       <c r="C26" s="22" t="s">
         <v>32</v>
       </c>
@@ -2082,7 +2083,7 @@
     </row>
     <row r="27" ht="18" customHeight="1" spans="1:7">
       <c r="A27" s="6"/>
-      <c r="B27" s="39"/>
+      <c r="B27" s="40"/>
       <c r="C27" s="22" t="s">
         <v>33</v>
       </c>
@@ -2090,14 +2091,14 @@
       <c r="E27" s="24">
         <v>1153846</v>
       </c>
-      <c r="F27" s="40" t="s">
+      <c r="F27" s="41" t="s">
         <v>27</v>
       </c>
       <c r="G27" s="8"/>
     </row>
     <row r="28" ht="18" customHeight="1" spans="1:7">
       <c r="A28" s="6"/>
-      <c r="B28" s="39"/>
+      <c r="B28" s="40"/>
       <c r="C28" s="22" t="s">
         <v>34</v>
       </c>
@@ -2105,14 +2106,14 @@
       <c r="E28" s="24">
         <v>240000</v>
       </c>
-      <c r="F28" s="40" t="s">
+      <c r="F28" s="41" t="s">
         <v>27</v>
       </c>
       <c r="G28" s="8"/>
     </row>
     <row r="29" ht="18" customHeight="1" spans="1:7">
       <c r="A29" s="6"/>
-      <c r="B29" s="39"/>
+      <c r="B29" s="40"/>
       <c r="C29" s="22" t="s">
         <v>35</v>
       </c>
@@ -2120,55 +2121,55 @@
       <c r="E29" s="24">
         <v>690000</v>
       </c>
-      <c r="F29" s="40" t="s">
+      <c r="F29" s="41" t="s">
         <v>27</v>
       </c>
       <c r="G29" s="8"/>
     </row>
     <row r="30" ht="18" customHeight="1" spans="1:7">
       <c r="A30" s="6"/>
-      <c r="B30" s="39"/>
+      <c r="B30" s="40"/>
       <c r="C30" s="22" t="s">
         <v>36</v>
       </c>
       <c r="D30" s="23"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="40" t="s">
+      <c r="E30" s="42"/>
+      <c r="F30" s="41" t="s">
         <v>27</v>
       </c>
       <c r="G30" s="8"/>
     </row>
     <row r="31" ht="18" customHeight="1" spans="1:7">
       <c r="A31" s="6"/>
-      <c r="B31" s="39"/>
-      <c r="C31" s="42" t="s">
+      <c r="B31" s="40"/>
+      <c r="C31" s="22" t="s">
         <v>37</v>
       </c>
       <c r="D31" s="43"/>
       <c r="E31" s="44"/>
-      <c r="F31" s="40" t="s">
+      <c r="F31" s="41" t="s">
         <v>27</v>
       </c>
       <c r="G31" s="8"/>
     </row>
     <row r="32" ht="18" customHeight="1" spans="1:7">
       <c r="A32" s="6"/>
-      <c r="B32" s="39"/>
-      <c r="C32" s="31" t="s">
+      <c r="B32" s="40"/>
+      <c r="C32" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="32"/>
+      <c r="D32" s="33"/>
       <c r="E32" s="45">
         <v>2545385</v>
       </c>
-      <c r="F32" s="40" t="s">
+      <c r="F32" s="41" t="s">
         <v>27</v>
       </c>
       <c r="G32" s="8"/>
     </row>
     <row r="33" ht="18" customHeight="1" spans="1:7">
       <c r="A33" s="6"/>
-      <c r="B33" s="39"/>
+      <c r="B33" s="40"/>
       <c r="C33" s="46" t="s">
         <v>39</v>
       </c>
@@ -2179,7 +2180,7 @@
     </row>
     <row r="34" ht="18" customHeight="1" spans="1:7">
       <c r="A34" s="6"/>
-      <c r="B34" s="39"/>
+      <c r="B34" s="40"/>
       <c r="C34" s="49" t="s">
         <v>40</v>
       </c>
@@ -2194,7 +2195,7 @@
     </row>
     <row r="35" ht="18" customHeight="1" spans="1:7">
       <c r="A35" s="6"/>
-      <c r="B35" s="39"/>
+      <c r="B35" s="40"/>
       <c r="C35" s="22" t="s">
         <v>41</v>
       </c>
@@ -2209,7 +2210,7 @@
     </row>
     <row r="36" ht="18" customHeight="1" spans="1:7">
       <c r="A36" s="6"/>
-      <c r="B36" s="39"/>
+      <c r="B36" s="40"/>
       <c r="C36" s="22" t="s">
         <v>43</v>
       </c>
@@ -2224,11 +2225,11 @@
     </row>
     <row r="37" ht="18" customHeight="1" spans="1:7">
       <c r="A37" s="6"/>
-      <c r="B37" s="39"/>
-      <c r="C37" s="31" t="s">
+      <c r="B37" s="40"/>
+      <c r="C37" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="D37" s="32"/>
+      <c r="D37" s="33"/>
       <c r="E37" s="55">
         <v>525000</v>
       </c>

</xml_diff>

<commit_message>
feat: add 2 row
</commit_message>
<xml_diff>
--- a/public/documents/payslip.xlsx
+++ b/public/documents/payslip.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000"/>
+    <workbookView windowWidth="23040" windowHeight="8280"/>
   </bookViews>
   <sheets>
     <sheet name="122025" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
   <si>
     <t>CÔNG TY TNHH HIGHWAN TECH VIETNAM</t>
   </si>
@@ -74,7 +74,7 @@
     <t>Nghỉ lễ, kết hôn, tang chế</t>
   </si>
   <si>
-    <t>Nghỉ phép năm</t>
+    <t>Số ngày nghỉ trong tháng</t>
   </si>
   <si>
     <t>Nghỉ ốm, Thai sản</t>
@@ -116,7 +116,7 @@
     <t>Hỗ trợ xăng xe, nhà ở</t>
   </si>
   <si>
-    <t>Tổng lương</t>
+    <t>Tổng lương (1)</t>
   </si>
   <si>
     <t>LƯƠNG, THUẾ</t>
@@ -137,13 +137,19 @@
     <t>Tổng tiền cơm trưa</t>
   </si>
   <si>
+    <t>Tiền phép năm</t>
+  </si>
+  <si>
+    <t>Tiền ngày lễ</t>
+  </si>
+  <si>
     <t>Phí gia công</t>
   </si>
   <si>
     <t>Thưởng Tết</t>
   </si>
   <si>
-    <t>Tổng thu nhập</t>
+    <t>Tổng thu nhập (2)</t>
   </si>
   <si>
     <t>Các khoảng khấu trừ</t>
@@ -161,10 +167,10 @@
     <t>Thuế TNCN</t>
   </si>
   <si>
-    <t>Tổng khấu trừ</t>
-  </si>
-  <si>
-    <t>Lương thực nhận</t>
+    <t>Tổng khấu trừ (3)</t>
+  </si>
+  <si>
+    <t>Lương thực nhận = (1) + (2) - (3)</t>
   </si>
   <si>
     <t>Người nhận</t>
@@ -1245,7 +1251,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1328,9 +1334,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="177" fontId="6" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="177" fontId="7" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1709,10 +1717,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -1796,7 +1804,7 @@
       <c r="C7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="11"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="8"/>
@@ -2129,11 +2137,11 @@
     <row r="30" ht="18" customHeight="1" spans="1:7">
       <c r="A30" s="6"/>
       <c r="B30" s="40"/>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="42" t="s">
         <v>36</v>
       </c>
       <c r="D30" s="23"/>
-      <c r="E30" s="42"/>
+      <c r="E30" s="43"/>
       <c r="F30" s="41" t="s">
         <v>27</v>
       </c>
@@ -2142,11 +2150,11 @@
     <row r="31" ht="18" customHeight="1" spans="1:7">
       <c r="A31" s="6"/>
       <c r="B31" s="40"/>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="43"/>
-      <c r="E31" s="44"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="43"/>
       <c r="F31" s="41" t="s">
         <v>27</v>
       </c>
@@ -2155,13 +2163,11 @@
     <row r="32" ht="18" customHeight="1" spans="1:7">
       <c r="A32" s="6"/>
       <c r="B32" s="40"/>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="33"/>
-      <c r="E32" s="45">
-        <v>2545385</v>
-      </c>
+      <c r="D32" s="23"/>
+      <c r="E32" s="44"/>
       <c r="F32" s="41" t="s">
         <v>27</v>
       </c>
@@ -2170,25 +2176,27 @@
     <row r="33" ht="18" customHeight="1" spans="1:7">
       <c r="A33" s="6"/>
       <c r="B33" s="40"/>
-      <c r="C33" s="46" t="s">
+      <c r="C33" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="48"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="41" t="s">
+        <v>27</v>
+      </c>
       <c r="G33" s="8"/>
     </row>
     <row r="34" ht="18" customHeight="1" spans="1:7">
       <c r="A34" s="6"/>
       <c r="B34" s="40"/>
-      <c r="C34" s="49" t="s">
+      <c r="C34" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="50"/>
-      <c r="E34" s="51">
-        <v>525000</v>
-      </c>
-      <c r="F34" s="52" t="s">
+      <c r="D34" s="33"/>
+      <c r="E34" s="47">
+        <v>2545385</v>
+      </c>
+      <c r="F34" s="41" t="s">
         <v>27</v>
       </c>
       <c r="G34" s="8"/>
@@ -2196,27 +2204,23 @@
     <row r="35" ht="18" customHeight="1" spans="1:7">
       <c r="A35" s="6"/>
       <c r="B35" s="40"/>
-      <c r="C35" s="22" t="s">
+      <c r="C35" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="23"/>
-      <c r="E35" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="F35" s="54" t="s">
-        <v>27</v>
-      </c>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="50"/>
       <c r="G35" s="8"/>
     </row>
     <row r="36" ht="18" customHeight="1" spans="1:7">
       <c r="A36" s="6"/>
       <c r="B36" s="40"/>
-      <c r="C36" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="D36" s="23"/>
-      <c r="E36" s="53" t="s">
+      <c r="C36" s="51" t="s">
         <v>42</v>
+      </c>
+      <c r="D36" s="52"/>
+      <c r="E36" s="53">
+        <v>525000</v>
       </c>
       <c r="F36" s="54" t="s">
         <v>27</v>
@@ -2226,12 +2230,12 @@
     <row r="37" ht="18" customHeight="1" spans="1:7">
       <c r="A37" s="6"/>
       <c r="B37" s="40"/>
-      <c r="C37" s="32" t="s">
+      <c r="C37" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" s="23"/>
+      <c r="E37" s="55" t="s">
         <v>44</v>
-      </c>
-      <c r="D37" s="33"/>
-      <c r="E37" s="55">
-        <v>525000</v>
       </c>
       <c r="F37" s="56" t="s">
         <v>27</v>
@@ -2240,80 +2244,110 @@
     </row>
     <row r="38" ht="18" customHeight="1" spans="1:7">
       <c r="A38" s="6"/>
-      <c r="B38" s="57"/>
-      <c r="C38" s="58" t="s">
+      <c r="B38" s="40"/>
+      <c r="C38" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="D38" s="59"/>
-      <c r="E38" s="60">
-        <f>E24+E32-E37</f>
-        <v>8020385</v>
-      </c>
-      <c r="F38" s="61" t="s">
+      <c r="D38" s="23"/>
+      <c r="E38" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="F38" s="56" t="s">
         <v>27</v>
       </c>
       <c r="G38" s="8"/>
     </row>
-    <row r="39" ht="10" customHeight="1" spans="1:7">
+    <row r="39" ht="18" customHeight="1" spans="1:7">
       <c r="A39" s="6"/>
-      <c r="B39" s="62"/>
-      <c r="C39" s="63"/>
-      <c r="D39" s="63"/>
-      <c r="E39" s="64"/>
-      <c r="F39" s="65"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="33"/>
+      <c r="E39" s="57">
+        <v>525000</v>
+      </c>
+      <c r="F39" s="58" t="s">
+        <v>27</v>
+      </c>
       <c r="G39" s="8"/>
     </row>
     <row r="40" ht="18" customHeight="1" spans="1:7">
       <c r="A40" s="6"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E40" s="7"/>
+      <c r="B40" s="59"/>
+      <c r="C40" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="D40" s="61"/>
+      <c r="E40" s="62">
+        <f>E24+E34-E39</f>
+        <v>8020385</v>
+      </c>
+      <c r="F40" s="63" t="s">
+        <v>27</v>
+      </c>
       <c r="G40" s="8"/>
     </row>
-    <row r="41" ht="18" customHeight="1" spans="1:7">
+    <row r="41" ht="10" customHeight="1" spans="1:7">
       <c r="A41" s="6"/>
-      <c r="C41" s="66"/>
-      <c r="D41" s="66" t="s">
-        <v>47</v>
-      </c>
+      <c r="B41" s="64"/>
+      <c r="C41" s="65"/>
+      <c r="D41" s="65"/>
       <c r="E41" s="66"/>
+      <c r="F41" s="67"/>
       <c r="G41" s="8"/>
     </row>
     <row r="42" ht="18" customHeight="1" spans="1:7">
       <c r="A42" s="6"/>
-      <c r="C42" s="67"/>
-      <c r="E42" s="67"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E42" s="7"/>
       <c r="G42" s="8"/>
     </row>
     <row r="43" ht="18" customHeight="1" spans="1:7">
       <c r="A43" s="6"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
+      <c r="C43" s="68"/>
+      <c r="D43" s="68" t="s">
+        <v>49</v>
+      </c>
+      <c r="E43" s="68"/>
       <c r="G43" s="8"/>
     </row>
     <row r="44" ht="18" customHeight="1" spans="1:7">
       <c r="A44" s="6"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7" t="s">
+      <c r="C44" s="69"/>
+      <c r="E44" s="69"/>
+      <c r="G44" s="8"/>
+    </row>
+    <row r="45" ht="18" customHeight="1" spans="1:7">
+      <c r="A45" s="6"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="G45" s="8"/>
+    </row>
+    <row r="46" ht="18" customHeight="1" spans="1:7">
+      <c r="A46" s="6"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E44" s="7"/>
-      <c r="G44" s="8"/>
-    </row>
-    <row r="45" ht="18" customHeight="1" spans="1:7">
-      <c r="A45" s="68"/>
-      <c r="B45" s="69"/>
-      <c r="C45" s="69"/>
-      <c r="D45" s="70"/>
-      <c r="E45" s="69"/>
-      <c r="F45" s="69"/>
-      <c r="G45" s="71"/>
+      <c r="E46" s="7"/>
+      <c r="G46" s="8"/>
+    </row>
+    <row r="47" ht="18" customHeight="1" spans="1:7">
+      <c r="A47" s="70"/>
+      <c r="B47" s="71"/>
+      <c r="C47" s="71"/>
+      <c r="D47" s="72"/>
+      <c r="E47" s="71"/>
+      <c r="F47" s="71"/>
+      <c r="G47" s="73"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="42">
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="C3:F3"/>
@@ -2343,17 +2377,19 @@
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="C33:D33"/>
     <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C35:F35"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D46:E46"/>
     <mergeCell ref="B9:B24"/>
-    <mergeCell ref="B25:B38"/>
+    <mergeCell ref="B25:B40"/>
   </mergeCells>
   <pageMargins left="0.25" right="0" top="0.25" bottom="0" header="0.3" footer="0.3"/>
   <pageSetup paperSize="11" scale="70" orientation="portrait"/>

</xml_diff>